<commit_message>
update pixel map excel
</commit_message>
<xml_diff>
--- a/Pixel Map.xlsx
+++ b/Pixel Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huakun Shen\Desktop\CSC258ProjectGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FE42637-076F-42CC-9F34-F4546B900AA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{45AC0085-41A1-41E1-BBF4-DE58276C7771}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19150" xr2:uid="{AA3D1601-B558-42BC-A8CC-A24BA5FFE2EB}"/>
   </bookViews>
@@ -43,7 +43,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -53,6 +53,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -86,7 +92,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -94,6 +100,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -410,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E848F5-5E40-4FA8-A593-1DCB8CF00166}">
-  <dimension ref="FE1"/>
+  <dimension ref="FE121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="ES35" sqref="ES35"/>
+      <selection activeCell="AO121" sqref="A121:XFD121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -422,7 +431,9 @@
     <col min="161" max="161" width="10.1640625" style="2" customWidth="1"/>
     <col min="162" max="16384" width="8.6640625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="121" s="3" customFormat="1"/>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added vga adapter files and some code
</commit_message>
<xml_diff>
--- a/Pixel Map.xlsx
+++ b/Pixel Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huakun Shen\Desktop\CSC258ProjectGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A3969F24-5E48-42C0-9683-84A31D04D52E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7110859-8A6A-407A-8382-CCA1BDE7A5B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19150" xr2:uid="{AA3D1601-B558-42BC-A8CC-A24BA5FFE2EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19150" xr2:uid="{AA3D1601-B558-42BC-A8CC-A24BA5FFE2EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,13 +421,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E848F5-5E40-4FA8-A593-1DCB8CF00166}">
   <dimension ref="FE121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="EB81" sqref="EB81"/>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="EM16" sqref="EM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="160" width="4.75" style="1" customWidth="1"/>
+    <col min="1" max="160" width="3.58203125" style="1" customWidth="1"/>
     <col min="161" max="161" width="10.1640625" style="2" customWidth="1"/>
     <col min="162" max="16384" width="8.6640625" style="1"/>
   </cols>

</xml_diff>